<commit_message>
update - progresbar, exeções, alertas modificados
Foi incluido um progress bar par melhor experiencia do usuario, tabem modificado os alertas das mensagens incluindo o de tratamento de exceções
</commit_message>
<xml_diff>
--- a/bases/planilha Base  OR copy.xlsx
+++ b/bases/planilha Base  OR copy.xlsx
@@ -54,7 +54,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +86,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -197,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -208,7 +214,7 @@
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -217,28 +223,25 @@
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -555,9 +558,9 @@
     <col min="1" max="1" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="13" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="15" width="82.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="15" width="26.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="82.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="26.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">

</xml_diff>

<commit_message>
Projeto fase 2 finalisado(gerar encomenda, gravar dados em banco de dados, gravar traking para etiqueta)
implementado a funçaõ para gerar encomendas no sistema da transportadora, onde a mesa retorna os código de encomneda, o código é gravado no sistema/pedido como tracking, possibilitando assim o volume ja sair todo identificado do armazem, incluindo tambem o salvamento altomatico em um banco de dados slite, outra funcionalidade e a consulta de uma encomenda gerar passando o numero da nota/ordem
</commit_message>
<xml_diff>
--- a/bases/planilha Base  OR copy.xlsx
+++ b/bases/planilha Base  OR copy.xlsx
@@ -54,7 +54,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,12 +86,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -223,7 +217,7 @@
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
@@ -563,7 +557,7 @@
     <col min="6" max="6" style="14" width="26.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +585,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="8">
-        <v>649739</v>
+        <v>653839</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>8</v>

</xml_diff>